<commit_message>
Holiday and Vacation add part working
Logic to add the printing a list of people who aren't working so that there is a "todo" list in the file.  Leaves off any entries on weekend or with no name.
</commit_message>
<xml_diff>
--- a/april.schedule.xlsx
+++ b/april.schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emst\Downloads\Personal\projects\python_practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C488E285-6ED8-4CE5-AD7E-3EEAB6AE7A7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5D3CDB-DEC7-43C5-AED7-E874A7E02B15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,23 +54,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Emmett Stewart:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-12hrs OT - Manpower coverage</t>
+          <t>12hrs OT - Manpower coverage</t>
         </r>
       </text>
     </comment>
@@ -228,7 +217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -317,13 +306,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -446,9 +428,6 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -507,6 +486,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -31363,7 +31345,7 @@
   <dimension ref="A1:AE17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75"/>
@@ -31373,1408 +31355,1408 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>2</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>3</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>5</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>6</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>7</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>8</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>9</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="5">
         <v>10</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="4">
         <v>11</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="4">
         <v>12</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="3">
         <v>13</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="3">
         <v>14</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="3">
         <v>15</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="3">
         <v>16</v>
       </c>
-      <c r="R2" s="4">
+      <c r="R2" s="3">
         <v>17</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="4">
         <v>18</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="4">
         <v>19</v>
       </c>
-      <c r="U2" s="4">
+      <c r="U2" s="3">
         <v>20</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="3">
         <v>21</v>
       </c>
-      <c r="W2" s="4">
+      <c r="W2" s="3">
         <v>22</v>
       </c>
-      <c r="X2" s="4">
+      <c r="X2" s="3">
         <v>23</v>
       </c>
-      <c r="Y2" s="4">
+      <c r="Y2" s="3">
         <v>24</v>
       </c>
-      <c r="Z2" s="5">
+      <c r="Z2" s="4">
         <v>25</v>
       </c>
-      <c r="AA2" s="5">
+      <c r="AA2" s="4">
         <v>26</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AB2" s="3">
         <v>27</v>
       </c>
-      <c r="AC2" s="4">
+      <c r="AC2" s="3">
         <v>28</v>
       </c>
-      <c r="AD2" s="4">
+      <c r="AD2" s="3">
         <v>29</v>
       </c>
-      <c r="AE2" s="4">
+      <c r="AE2" s="3">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:31">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="8" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="8" t="s">
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="Q3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="R3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="8" t="s">
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="V3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="W3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="X3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Y3" s="8" t="s">
+      <c r="Y3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="8" t="s">
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="8" t="s">
+      <c r="AC3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AD3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AE3" s="8" t="s">
+      <c r="AE3" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:31">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="11" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="11" t="s">
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="11" t="s">
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="11" t="s">
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="S4" s="12" t="s">
+      <c r="S4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="T4" s="9"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="11" t="s">
+      <c r="T4" s="8"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="W4" s="12" t="s">
+      <c r="W4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="11" t="s">
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AA4" s="12" t="s">
+      <c r="AA4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="11" t="s">
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="11" t="s">
+      <c r="AD4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AE4" s="14" t="s">
+      <c r="AE4" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:31">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="11" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="11" t="s">
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="9"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="11" t="s">
+      <c r="M5" s="8"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="P5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="11" t="s">
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="T5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="11" t="s">
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="X5" s="12" t="s">
+      <c r="X5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="11" t="s">
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AB5" s="12" t="s">
+      <c r="AB5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="11" t="s">
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="12"/>
+      <c r="AE5" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:31">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="11" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="11" t="s">
+      <c r="F6" s="8"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="11" t="s">
+      <c r="J6" s="12"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="O6" s="13"/>
-      <c r="P6" s="11" t="s">
+      <c r="O6" s="12"/>
+      <c r="P6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="12" t="s">
+      <c r="Q6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="R6" s="13"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="11" t="s">
+      <c r="R6" s="12"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="U6" s="12" t="s">
+      <c r="U6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="11" t="s">
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Y6" s="12" t="s">
+      <c r="Y6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="11" t="s">
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AC6" s="12" t="s">
+      <c r="AC6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="13"/>
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="12"/>
     </row>
     <row r="7" spans="1:31">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="11" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="11" t="s">
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="15"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="11" t="s">
+      <c r="K7" s="14"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="N7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="11" t="s">
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="R7" s="12" t="s">
+      <c r="R7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="11" t="s">
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="V7" s="12" t="s">
+      <c r="V7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="11" t="s">
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Z7" s="12" t="s">
+      <c r="Z7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="11" t="s">
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AD7" s="12" t="s">
+      <c r="AD7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AE7" s="13"/>
+      <c r="AE7" s="12"/>
     </row>
     <row r="8" spans="1:31">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="11" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="11" t="s">
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="11" t="s">
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="O8" s="12" t="s">
+      <c r="O8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="11" t="s">
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="S8" s="12" t="s">
+      <c r="S8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="T8" s="9"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="11" t="s">
+      <c r="T8" s="8"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="W8" s="12" t="s">
+      <c r="W8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="11" t="s">
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AA8" s="12" t="s">
+      <c r="AA8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="13"/>
-      <c r="AD8" s="11" t="s">
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AE8" s="17" t="s">
+      <c r="AE8" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:31">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="11" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="11" t="s">
+      <c r="F9" s="8"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="11" t="s">
+      <c r="J9" s="12"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="11" t="s">
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Q9" s="11" t="s">
+      <c r="Q9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="R9" s="13"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="11" t="s">
+      <c r="R9" s="12"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="U9" s="11" t="s">
+      <c r="U9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="11" t="s">
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Y9" s="11" t="s">
+      <c r="Y9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Z9" s="9"/>
-      <c r="AA9" s="9"/>
-      <c r="AB9" s="11" t="s">
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AC9" s="11" t="s">
+      <c r="AC9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AD9" s="18" t="s">
+      <c r="AD9" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="AE9" s="18" t="s">
+      <c r="AE9" s="17" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:31">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="8" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="8" t="s">
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="O10" s="8" t="s">
+      <c r="O10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="P10" s="8" t="s">
+      <c r="P10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Q10" s="8" t="s">
+      <c r="Q10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R10" s="8" t="s">
+      <c r="R10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="19" t="s">
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="V10" s="19" t="s">
+      <c r="V10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="W10" s="19" t="s">
+      <c r="W10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="X10" s="19" t="s">
+      <c r="X10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="Y10" s="19" t="s">
+      <c r="Y10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="9"/>
-      <c r="AB10" s="19" t="s">
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="AC10" s="19" t="s">
+      <c r="AC10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="AD10" s="19" t="s">
+      <c r="AD10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="AE10" s="19" t="s">
+      <c r="AE10" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:31">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="K11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="21" t="s">
+      <c r="L11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="21" t="s">
+      <c r="M11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="21" t="s">
+      <c r="N11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="O11" s="21" t="s">
+      <c r="O11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="P11" s="21" t="s">
+      <c r="P11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="Q11" s="20" t="s">
+      <c r="Q11" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="R11" s="20" t="s">
+      <c r="R11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="S11" s="20" t="s">
+      <c r="S11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="T11" s="21" t="s">
+      <c r="T11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="U11" s="21" t="s">
+      <c r="U11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="V11" s="20" t="s">
+      <c r="V11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="W11" s="20" t="s">
+      <c r="W11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="X11" s="21" t="s">
+      <c r="X11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Y11" s="21" t="s">
+      <c r="Y11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="Z11" s="20" t="s">
+      <c r="Z11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AA11" s="20" t="s">
+      <c r="AA11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AB11" s="21" t="s">
+      <c r="AB11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="AC11" s="22" t="s">
+      <c r="AC11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AD11" s="20" t="s">
+      <c r="AD11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AE11" s="20" t="s">
+      <c r="AE11" s="19" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:31">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="J12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="20" t="s">
+      <c r="K12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="21" t="s">
+      <c r="L12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="21" t="s">
+      <c r="M12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="21" t="s">
+      <c r="N12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="O12" s="21" t="s">
+      <c r="O12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="P12" s="21" t="s">
+      <c r="P12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="Q12" s="20" t="s">
+      <c r="Q12" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="R12" s="20" t="s">
+      <c r="R12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="S12" s="20" t="s">
+      <c r="S12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="T12" s="21" t="s">
+      <c r="T12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="U12" s="21" t="s">
+      <c r="U12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="V12" s="20" t="s">
+      <c r="V12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="W12" s="20" t="s">
+      <c r="W12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="X12" s="21" t="s">
+      <c r="X12" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Y12" s="21" t="s">
+      <c r="Y12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="Z12" s="20" t="s">
+      <c r="Z12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AA12" s="20" t="s">
+      <c r="AA12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AB12" s="19" t="s">
+      <c r="AB12" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="AC12" s="19" t="s">
+      <c r="AC12" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="AD12" s="19" t="s">
+      <c r="AD12" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="AE12" s="19" t="s">
+      <c r="AE12" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:31">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="21" t="s">
+      <c r="K13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="21" t="s">
+      <c r="L13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M13" s="20" t="s">
+      <c r="M13" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="N13" s="20" t="s">
+      <c r="N13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="20" t="s">
+      <c r="O13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="P13" s="21" t="s">
+      <c r="P13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="Q13" s="21" t="s">
+      <c r="Q13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="R13" s="20" t="s">
+      <c r="R13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="S13" s="20" t="s">
+      <c r="S13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="T13" s="21" t="s">
+      <c r="T13" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="U13" s="21" t="s">
+      <c r="U13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="V13" s="20" t="s">
+      <c r="V13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="W13" s="20" t="s">
+      <c r="W13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="X13" s="21" t="s">
+      <c r="X13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="Y13" s="22" t="s">
+      <c r="Y13" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="Z13" s="20" t="s">
+      <c r="Z13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AA13" s="20" t="s">
+      <c r="AA13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AB13" s="21" t="s">
+      <c r="AB13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="AC13" s="22" t="s">
+      <c r="AC13" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AD13" s="20" t="s">
+      <c r="AD13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AE13" s="20" t="s">
+      <c r="AE13" s="19" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:31">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="J14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="K14" s="20" t="s">
+      <c r="K14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="L14" s="21" t="s">
+      <c r="L14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M14" s="21" t="s">
+      <c r="M14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="21" t="s">
+      <c r="N14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="O14" s="21" t="s">
+      <c r="O14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="P14" s="21" t="s">
+      <c r="P14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="Q14" s="20" t="s">
+      <c r="Q14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="R14" s="20" t="s">
+      <c r="R14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="S14" s="20" t="s">
+      <c r="S14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="T14" s="21" t="s">
+      <c r="T14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="U14" s="21" t="s">
+      <c r="U14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="V14" s="20" t="s">
+      <c r="V14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="W14" s="20" t="s">
+      <c r="W14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="X14" s="21" t="s">
+      <c r="X14" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Y14" s="21" t="s">
+      <c r="Y14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="Z14" s="20" t="s">
+      <c r="Z14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AA14" s="20" t="s">
+      <c r="AA14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AB14" s="21" t="s">
+      <c r="AB14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="AC14" s="22" t="s">
+      <c r="AC14" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AD14" s="20" t="s">
+      <c r="AD14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AE14" s="20" t="s">
+      <c r="AE14" s="19" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:31">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="21" t="s">
+      <c r="I15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="J15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="K15" s="20" t="s">
+      <c r="K15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="21" t="s">
+      <c r="L15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M15" s="21" t="s">
+      <c r="M15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="21" t="s">
+      <c r="N15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="O15" s="21" t="s">
+      <c r="O15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="P15" s="21" t="s">
+      <c r="P15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="Q15" s="20" t="s">
+      <c r="Q15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="R15" s="20" t="s">
+      <c r="R15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="S15" s="20" t="s">
+      <c r="S15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="T15" s="21" t="s">
+      <c r="T15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="U15" s="21" t="s">
+      <c r="U15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="V15" s="20" t="s">
+      <c r="V15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="W15" s="20" t="s">
+      <c r="W15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="X15" s="21" t="s">
+      <c r="X15" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Y15" s="21" t="s">
+      <c r="Y15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="Z15" s="20" t="s">
+      <c r="Z15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AA15" s="20" t="s">
+      <c r="AA15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AB15" s="21" t="s">
+      <c r="AB15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="AC15" s="22" t="s">
+      <c r="AC15" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AD15" s="20" t="s">
+      <c r="AD15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AE15" s="20" t="s">
+      <c r="AE15" s="19" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:31">
-      <c r="A16" s="16"/>
-      <c r="B16" s="23">
+      <c r="A16" s="15"/>
+      <c r="B16" s="22">
         <f t="array" ref="B16">(COUNTIF(B1:B10,"D")*100)+((COUNTIF(B1:B10,"2D")*100))+((COUNTIF(B1:B10,"N")*10))+((COUNTIF(B1:B10,"2N")*10))+((COUNTIF(B1:B10,"D2")*1))+((COUNTIF(B1:B10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="22">
         <f t="array" ref="C16">(COUNTIF(C1:C10,"D")*100)+((COUNTIF(C1:C10,"2D")*100))+((COUNTIF(C1:C10,"N")*10))+((COUNTIF(C1:C10,"2N")*10))+((COUNTIF(C1:C10,"D2")*1))+((COUNTIF(C1:C10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="22">
         <f t="array" ref="D16">(COUNTIF(D1:D10,"D")*100)+((COUNTIF(D1:D10,"2D")*100))+((COUNTIF(D1:D10,"N")*10))+((COUNTIF(D1:D10,"2N")*10))+((COUNTIF(D1:D10,"D2")*1))+((COUNTIF(D1:D10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="22">
         <f t="array" ref="E16">(COUNTIF(E1:E10,"D")*100)+((COUNTIF(E1:E10,"2D")*100))+((COUNTIF(E1:E10,"N")*10))+((COUNTIF(E1:E10,"2N")*10))+((COUNTIF(E1:E10,"D2")*1))+((COUNTIF(E1:E10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="22">
         <f t="array" ref="F16">(COUNTIF(F1:F10,"D")*100)+((COUNTIF(F1:F10,"2D")*100))+((COUNTIF(F1:F10,"N")*10))+((COUNTIF(F1:F10,"2N")*10))+((COUNTIF(F1:F10,"D2")*1))+((COUNTIF(F1:F10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="22">
         <f t="array" ref="G16">(COUNTIF(G1:G10,"D")*100)+((COUNTIF(G1:G10,"2D")*100))+((COUNTIF(G1:G10,"N")*10))+((COUNTIF(G1:G10,"2N")*10))+((COUNTIF(G1:G10,"D2")*1))+((COUNTIF(G1:G10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="22">
         <f t="array" ref="H16">(COUNTIF(H1:H10,"D")*100)+((COUNTIF(H1:H10,"2D")*100))+((COUNTIF(H1:H10,"N")*10))+((COUNTIF(H1:H10,"2N")*10))+((COUNTIF(H1:H10,"D2")*1))+((COUNTIF(H1:H10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="I16" s="23">
+      <c r="I16" s="22">
         <f t="array" ref="I16">(COUNTIF(I1:I10,"D")*100)+((COUNTIF(I1:I10,"2D")*100))+((COUNTIF(I1:I10,"N")*10))+((COUNTIF(I1:I10,"2N")*10))+((COUNTIF(I1:I10,"D2")*1))+((COUNTIF(I1:I10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="J16" s="23">
+      <c r="J16" s="22">
         <f t="array" ref="J16">(COUNTIF(J1:J10,"D")*100)+((COUNTIF(J1:J10,"2D")*100))+((COUNTIF(J1:J10,"N")*10))+((COUNTIF(J1:J10,"2N")*10))+((COUNTIF(J1:J10,"D2")*1))+((COUNTIF(J1:J10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="K16" s="23">
+      <c r="K16" s="22">
         <f t="array" ref="K16">(COUNTIF(K1:K10,"D")*100)+((COUNTIF(K1:K10,"2D")*100))+((COUNTIF(K1:K10,"N")*10))+((COUNTIF(K1:K10,"2N")*10))+((COUNTIF(K1:K10,"D2")*1))+((COUNTIF(K1:K10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="L16" s="23">
+      <c r="L16" s="22">
         <f t="array" ref="L16">(COUNTIF(L1:L10,"D")*100)+((COUNTIF(L1:L10,"2D")*100))+((COUNTIF(L1:L10,"N")*10))+((COUNTIF(L1:L10,"2N")*10))+((COUNTIF(L1:L10,"D2")*1))+((COUNTIF(L1:L10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="M16" s="23">
+      <c r="M16" s="22">
         <f t="array" ref="M16">(COUNTIF(M1:M10,"D")*100)+((COUNTIF(M1:M10,"2D")*100))+((COUNTIF(M1:M10,"N")*10))+((COUNTIF(M1:M10,"2N")*10))+((COUNTIF(M1:M10,"D2")*1))+((COUNTIF(M1:M10,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="N16" s="23">
+      <c r="N16" s="22">
         <f t="array" ref="N16">(COUNTIF(N1:N10,"D")*100)+((COUNTIF(N1:N10,"2D")*100))+((COUNTIF(N1:N10,"N")*10))+((COUNTIF(N1:N10,"2N")*10))+((COUNTIF(N1:N10,"D2")*1))+((COUNTIF(N1:N10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="O16" s="23">
+      <c r="O16" s="22">
         <f t="array" ref="O16">(COUNTIF(O1:O10,"D")*100)+((COUNTIF(O1:O10,"2D")*100))+((COUNTIF(O1:O10,"N")*10))+((COUNTIF(O1:O10,"2N")*10))+((COUNTIF(O1:O10,"D2")*1))+((COUNTIF(O1:O10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="P16" s="23">
+      <c r="P16" s="22">
         <f t="array" ref="P16">(COUNTIF(P1:P10,"D")*100)+((COUNTIF(P1:P10,"2D")*100))+((COUNTIF(P1:P10,"N")*10))+((COUNTIF(P1:P10,"2N")*10))+((COUNTIF(P1:P10,"D2")*1))+((COUNTIF(P1:P10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="Q16" s="23">
+      <c r="Q16" s="22">
         <f t="array" ref="Q16">(COUNTIF(Q1:Q10,"D")*100)+((COUNTIF(Q1:Q10,"2D")*100))+((COUNTIF(Q1:Q10,"N")*10))+((COUNTIF(Q1:Q10,"2N")*10))+((COUNTIF(Q1:Q10,"D2")*1))+((COUNTIF(Q1:Q10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="R16" s="23">
+      <c r="R16" s="22">
         <f t="array" ref="R16">(COUNTIF(R1:R10,"D")*100)+((COUNTIF(R1:R10,"2D")*100))+((COUNTIF(R1:R10,"N")*10))+((COUNTIF(R1:R10,"2N")*10))+((COUNTIF(R1:R10,"D2")*1))+((COUNTIF(R1:R10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="S16" s="23">
+      <c r="S16" s="22">
         <f t="array" ref="S16">(COUNTIF(S1:S10,"D")*100)+((COUNTIF(S1:S10,"2D")*100))+((COUNTIF(S1:S10,"N")*10))+((COUNTIF(S1:S10,"2N")*10))+((COUNTIF(S1:S10,"D2")*1))+((COUNTIF(S1:S10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="T16" s="23">
+      <c r="T16" s="22">
         <f t="array" ref="T16">(COUNTIF(T1:T10,"D")*100)+((COUNTIF(T1:T10,"2D")*100))+((COUNTIF(T1:T10,"N")*10))+((COUNTIF(T1:T10,"2N")*10))+((COUNTIF(T1:T10,"D2")*1))+((COUNTIF(T1:T10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="U16" s="23">
+      <c r="U16" s="22">
         <f t="array" ref="U16">(COUNTIF(U1:U10,"D")*100)+((COUNTIF(U1:U10,"2D")*100))+((COUNTIF(U1:U10,"N")*10))+((COUNTIF(U1:U10,"2N")*10))+((COUNTIF(U1:U10,"D2")*1))+((COUNTIF(U1:U10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="V16" s="23">
+      <c r="V16" s="22">
         <f t="array" ref="V16">(COUNTIF(V1:V10,"D")*100)+((COUNTIF(V1:V10,"2D")*100))+((COUNTIF(V1:V10,"N")*10))+((COUNTIF(V1:V10,"2N")*10))+((COUNTIF(V1:V10,"D2")*1))+((COUNTIF(V1:V10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="W16" s="23">
+      <c r="W16" s="22">
         <f t="array" ref="W16">(COUNTIF(W1:W10,"D")*100)+((COUNTIF(W1:W10,"2D")*100))+((COUNTIF(W1:W10,"N")*10))+((COUNTIF(W1:W10,"2N")*10))+((COUNTIF(W1:W10,"D2")*1))+((COUNTIF(W1:W10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="X16" s="23">
+      <c r="X16" s="22">
         <f t="array" ref="X16">(COUNTIF(X1:X10,"D")*100)+((COUNTIF(X1:X10,"2D")*100))+((COUNTIF(X1:X10,"N")*10))+((COUNTIF(X1:X10,"2N")*10))+((COUNTIF(X1:X10,"D2")*1))+((COUNTIF(X1:X10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="Y16" s="23">
+      <c r="Y16" s="22">
         <f t="array" ref="Y16">(COUNTIF(Y1:Y10,"D")*100)+((COUNTIF(Y1:Y10,"2D")*100))+((COUNTIF(Y1:Y10,"N")*10))+((COUNTIF(Y1:Y10,"2N")*10))+((COUNTIF(Y1:Y10,"D2")*1))+((COUNTIF(Y1:Y10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="Z16" s="23">
+      <c r="Z16" s="22">
         <f t="array" ref="Z16">(COUNTIF(Z1:Z10,"D")*100)+((COUNTIF(Z1:Z10,"2D")*100))+((COUNTIF(Z1:Z10,"N")*10))+((COUNTIF(Z1:Z10,"2N")*10))+((COUNTIF(Z1:Z10,"D2")*1))+((COUNTIF(Z1:Z10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="AA16" s="23">
+      <c r="AA16" s="22">
         <f t="array" ref="AA16">(COUNTIF(AA1:AA10,"D")*100)+((COUNTIF(AA1:AA10,"2D")*100))+((COUNTIF(AA1:AA10,"N")*10))+((COUNTIF(AA1:AA10,"2N")*10))+((COUNTIF(AA1:AA10,"D2")*1))+((COUNTIF(AA1:AA10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="AB16" s="23">
+      <c r="AB16" s="22">
         <f t="array" ref="AB16">(COUNTIF(AB1:AB10,"D")*100)+((COUNTIF(AB1:AB10,"2D")*100))+((COUNTIF(AB1:AB10,"N")*10))+((COUNTIF(AB1:AB10,"2N")*10))+((COUNTIF(AB1:AB10,"D2")*1))+((COUNTIF(AB1:AB10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="AC16" s="23">
+      <c r="AC16" s="22">
         <f t="array" ref="AC16">(COUNTIF(AC1:AC10,"D")*100)+((COUNTIF(AC1:AC10,"2D")*100))+((COUNTIF(AC1:AC10,"N")*10))+((COUNTIF(AC1:AC10,"2N")*10))+((COUNTIF(AC1:AC10,"D2")*1))+((COUNTIF(AC1:AC10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="AD16" s="23">
+      <c r="AD16" s="22">
         <f t="array" ref="AD16">(COUNTIF(AD1:AD10,"D")*100)+((COUNTIF(AD1:AD10,"2D")*100))+((COUNTIF(AD1:AD10,"N")*10))+((COUNTIF(AD1:AD10,"2N")*10))+((COUNTIF(AD1:AD10,"D2")*1))+((COUNTIF(AD1:AD10,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="AE16" s="23">
+      <c r="AE16" s="22">
         <f t="array" ref="AE16">(COUNTIF(AE1:AE10,"D")*100)+((COUNTIF(AE1:AE10,"2D")*100))+((COUNTIF(AE1:AE10,"N")*10))+((COUNTIF(AE1:AE10,"2N")*10))+((COUNTIF(AE1:AE10,"D2")*1))+((COUNTIF(AE1:AE10,"2D2")*1))</f>
         <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:31">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25">
+      <c r="A17" s="23"/>
+      <c r="B17" s="24">
         <f t="array" ref="B17">(COUNTIF(B3:B7,"D")*100)+((COUNTIF(B3:B7,"N")*10))+((COUNTIF(B3:B7,"D2")*1))+((COUNTIF(B3:B7,"2D")*100))+((COUNTIF(B3:B7,"2N")*10))+((COUNTIF(B3:B7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="24">
         <f t="array" ref="C17">(COUNTIF(C3:C7,"D")*100)+((COUNTIF(C3:C7,"N")*10))+((COUNTIF(C3:C7,"D2")*1))+((COUNTIF(C3:C7,"2D")*100))+((COUNTIF(C3:C7,"2N")*10))+((COUNTIF(C3:C7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="24">
         <f t="array" ref="D17">(COUNTIF(D3:D7,"D")*100)+((COUNTIF(D3:D7,"N")*10))+((COUNTIF(D3:D7,"D2")*1))+((COUNTIF(D3:D7,"2D")*100))+((COUNTIF(D3:D7,"2N")*10))+((COUNTIF(D3:D7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="24">
         <f t="array" ref="E17">(COUNTIF(E3:E7,"D")*100)+((COUNTIF(E3:E7,"N")*10))+((COUNTIF(E3:E7,"D2")*1))+((COUNTIF(E3:E7,"2D")*100))+((COUNTIF(E3:E7,"2N")*10))+((COUNTIF(E3:E7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="24">
         <f t="array" ref="F17">(COUNTIF(F3:F7,"D")*100)+((COUNTIF(F3:F7,"N")*10))+((COUNTIF(F3:F7,"D2")*1))+((COUNTIF(F3:F7,"2D")*100))+((COUNTIF(F3:F7,"2N")*10))+((COUNTIF(F3:F7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="24">
         <f t="array" ref="G17">(COUNTIF(G3:G7,"D")*100)+((COUNTIF(G3:G7,"N")*10))+((COUNTIF(G3:G7,"D2")*1))+((COUNTIF(G3:G7,"2D")*100))+((COUNTIF(G3:G7,"2N")*10))+((COUNTIF(G3:G7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="24">
         <f t="array" ref="H17">(COUNTIF(H3:H7,"D")*100)+((COUNTIF(H3:H7,"N")*10))+((COUNTIF(H3:H7,"D2")*1))+((COUNTIF(H3:H7,"2D")*100))+((COUNTIF(H3:H7,"2N")*10))+((COUNTIF(H3:H7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="24">
         <f t="array" ref="I17">(COUNTIF(I3:I7,"D")*100)+((COUNTIF(I3:I7,"N")*10))+((COUNTIF(I3:I7,"D2")*1))+((COUNTIF(I3:I7,"2D")*100))+((COUNTIF(I3:I7,"2N")*10))+((COUNTIF(I3:I7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="J17" s="25">
+      <c r="J17" s="24">
         <f t="array" ref="J17">(COUNTIF(J3:J7,"D")*100)+((COUNTIF(J3:J7,"N")*10))+((COUNTIF(J3:J7,"D2")*1))+((COUNTIF(J3:J7,"2D")*100))+((COUNTIF(J3:J7,"2N")*10))+((COUNTIF(J3:J7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="24">
         <f t="array" ref="K17">(COUNTIF(K3:K7,"D")*100)+((COUNTIF(K3:K7,"N")*10))+((COUNTIF(K3:K7,"D2")*1))+((COUNTIF(K3:K7,"2D")*100))+((COUNTIF(K3:K7,"2N")*10))+((COUNTIF(K3:K7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17" s="24">
         <f t="array" ref="L17">(COUNTIF(L3:L7,"D")*100)+((COUNTIF(L3:L7,"N")*10))+((COUNTIF(L3:L7,"D2")*1))+((COUNTIF(L3:L7,"2D")*100))+((COUNTIF(L3:L7,"2N")*10))+((COUNTIF(L3:L7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="24">
         <f t="array" ref="M17">(COUNTIF(M3:M7,"D")*100)+((COUNTIF(M3:M7,"N")*10))+((COUNTIF(M3:M7,"D2")*1))+((COUNTIF(M3:M7,"2D")*100))+((COUNTIF(M3:M7,"2N")*10))+((COUNTIF(M3:M7,"2D2")*1))</f>
         <v>10</v>
       </c>
-      <c r="N17" s="25">
+      <c r="N17" s="24">
         <f t="array" ref="N17">(COUNTIF(N3:N7,"D")*100)+((COUNTIF(N3:N7,"N")*10))+((COUNTIF(N3:N7,"D2")*1))+((COUNTIF(N3:N7,"2D")*100))+((COUNTIF(N3:N7,"2N")*10))+((COUNTIF(N3:N7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="O17" s="25">
+      <c r="O17" s="24">
         <f t="array" ref="O17">(COUNTIF(O3:O7,"D")*100)+((COUNTIF(O3:O7,"N")*10))+((COUNTIF(O3:O7,"D2")*1))+((COUNTIF(O3:O7,"2D")*100))+((COUNTIF(O3:O7,"2N")*10))+((COUNTIF(O3:O7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="P17" s="25">
+      <c r="P17" s="24">
         <f t="array" ref="P17">(COUNTIF(P3:P7,"D")*100)+((COUNTIF(P3:P7,"N")*10))+((COUNTIF(P3:P7,"D2")*1))+((COUNTIF(P3:P7,"2D")*100))+((COUNTIF(P3:P7,"2N")*10))+((COUNTIF(P3:P7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="Q17" s="25">
+      <c r="Q17" s="24">
         <f t="array" ref="Q17">(COUNTIF(Q3:Q7,"D")*100)+((COUNTIF(Q3:Q7,"N")*10))+((COUNTIF(Q3:Q7,"D2")*1))+((COUNTIF(Q3:Q7,"2D")*100))+((COUNTIF(Q3:Q7,"2N")*10))+((COUNTIF(Q3:Q7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="R17" s="25">
+      <c r="R17" s="24">
         <f t="array" ref="R17">(COUNTIF(R3:R7,"D")*100)+((COUNTIF(R3:R7,"N")*10))+((COUNTIF(R3:R7,"D2")*1))+((COUNTIF(R3:R7,"2D")*100))+((COUNTIF(R3:R7,"2N")*10))+((COUNTIF(R3:R7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="S17" s="25">
+      <c r="S17" s="24">
         <f t="array" ref="S17">(COUNTIF(S3:S7,"D")*100)+((COUNTIF(S3:S7,"N")*10))+((COUNTIF(S3:S7,"D2")*1))+((COUNTIF(S3:S7,"2D")*100))+((COUNTIF(S3:S7,"2N")*10))+((COUNTIF(S3:S7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="T17" s="25">
+      <c r="T17" s="24">
         <f t="array" ref="T17">(COUNTIF(T3:T7,"D")*100)+((COUNTIF(T3:T7,"N")*10))+((COUNTIF(T3:T7,"D2")*1))+((COUNTIF(T3:T7,"2D")*100))+((COUNTIF(T3:T7,"2N")*10))+((COUNTIF(T3:T7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="U17" s="25">
+      <c r="U17" s="24">
         <f t="array" ref="U17">(COUNTIF(U3:U7,"D")*100)+((COUNTIF(U3:U7,"N")*10))+((COUNTIF(U3:U7,"D2")*1))+((COUNTIF(U3:U7,"2D")*100))+((COUNTIF(U3:U7,"2N")*10))+((COUNTIF(U3:U7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="V17" s="25">
+      <c r="V17" s="24">
         <f t="array" ref="V17">(COUNTIF(V3:V7,"D")*100)+((COUNTIF(V3:V7,"N")*10))+((COUNTIF(V3:V7,"D2")*1))+((COUNTIF(V3:V7,"2D")*100))+((COUNTIF(V3:V7,"2N")*10))+((COUNTIF(V3:V7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="W17" s="25">
+      <c r="W17" s="24">
         <f t="array" ref="W17">(COUNTIF(W3:W7,"D")*100)+((COUNTIF(W3:W7,"N")*10))+((COUNTIF(W3:W7,"D2")*1))+((COUNTIF(W3:W7,"2D")*100))+((COUNTIF(W3:W7,"2N")*10))+((COUNTIF(W3:W7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="X17" s="25">
+      <c r="X17" s="24">
         <f t="array" ref="X17">(COUNTIF(X3:X7,"D")*100)+((COUNTIF(X3:X7,"N")*10))+((COUNTIF(X3:X7,"D2")*1))+((COUNTIF(X3:X7,"2D")*100))+((COUNTIF(X3:X7,"2N")*10))+((COUNTIF(X3:X7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="Y17" s="25">
+      <c r="Y17" s="24">
         <f t="array" ref="Y17">(COUNTIF(Y3:Y7,"D")*100)+((COUNTIF(Y3:Y7,"N")*10))+((COUNTIF(Y3:Y7,"D2")*1))+((COUNTIF(Y3:Y7,"2D")*100))+((COUNTIF(Y3:Y7,"2N")*10))+((COUNTIF(Y3:Y7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="Z17" s="25">
+      <c r="Z17" s="24">
         <f t="array" ref="Z17">(COUNTIF(Z3:Z7,"D")*100)+((COUNTIF(Z3:Z7,"N")*10))+((COUNTIF(Z3:Z7,"D2")*1))+((COUNTIF(Z3:Z7,"2D")*100))+((COUNTIF(Z3:Z7,"2N")*10))+((COUNTIF(Z3:Z7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="AA17" s="25">
+      <c r="AA17" s="24">
         <f t="array" ref="AA17">(COUNTIF(AA3:AA7,"D")*100)+((COUNTIF(AA3:AA7,"N")*10))+((COUNTIF(AA3:AA7,"D2")*1))+((COUNTIF(AA3:AA7,"2D")*100))+((COUNTIF(AA3:AA7,"2N")*10))+((COUNTIF(AA3:AA7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="AB17" s="25">
+      <c r="AB17" s="24">
         <f t="array" ref="AB17">(COUNTIF(AB3:AB7,"D")*100)+((COUNTIF(AB3:AB7,"N")*10))+((COUNTIF(AB3:AB7,"D2")*1))+((COUNTIF(AB3:AB7,"2D")*100))+((COUNTIF(AB3:AB7,"2N")*10))+((COUNTIF(AB3:AB7,"2D2")*1))</f>
         <v>200</v>
       </c>
-      <c r="AC17" s="25">
+      <c r="AC17" s="24">
         <f t="array" ref="AC17">(COUNTIF(AC3:AC7,"D")*100)+((COUNTIF(AC3:AC7,"N")*10))+((COUNTIF(AC3:AC7,"D2")*1))+((COUNTIF(AC3:AC7,"2D")*100))+((COUNTIF(AC3:AC7,"2N")*10))+((COUNTIF(AC3:AC7,"2D2")*1))</f>
         <v>210</v>
       </c>
-      <c r="AD17" s="25">
+      <c r="AD17" s="24">
         <f t="array" ref="AD17">(COUNTIF(AD3:AD7,"D")*100)+((COUNTIF(AD3:AD7,"N")*10))+((COUNTIF(AD3:AD7,"D2")*1))+((COUNTIF(AD3:AD7,"2D")*100))+((COUNTIF(AD3:AD7,"2N")*10))+((COUNTIF(AD3:AD7,"2D2")*1))</f>
         <v>110</v>
       </c>
-      <c r="AE17" s="25">
+      <c r="AE17" s="24">
         <f t="array" ref="AE17">(COUNTIF(AE3:AE7,"D")*100)+((COUNTIF(AE3:AE7,"N")*10))+((COUNTIF(AE3:AE7,"D2")*1))+((COUNTIF(AE3:AE7,"2D")*100))+((COUNTIF(AE3:AE7,"2N")*10))+((COUNTIF(AE3:AE7,"2D2")*1))</f>
         <v>200</v>
       </c>

</xml_diff>